<commit_message>
Improvements on Technical Work
On 5 of February 2021, Feed Forward Neural Network and Convolutional Neural Network were implemented and used with Fruits-360 dataset in this project.
</commit_message>
<xml_diff>
--- a/Records of Technical Work.xlsx
+++ b/Records of Technical Work.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>DATE</t>
   </si>
@@ -45,6 +45,12 @@
   </si>
   <si>
     <t>Uploaded all the datasets into Google Drive and decided to use Pytorch library for the project</t>
+  </si>
+  <si>
+    <t>Implemented Feed Forward Neural Network model and Convolutional Neural Network. The Feed Forward Neural Network achieved final accuracy of 88.69% on Fruits-360 dataset. Whereas, Convolutional Neural Network achieved accuracy of 95% on Fruits-360 dataset.</t>
+  </si>
+  <si>
+    <t>Apply different algorithms to the Fruits-360 dataset and also combine Fruits-360 dataset with another dataset (waste), to see the results.</t>
   </si>
 </sst>
 </file>
@@ -117,7 +123,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -127,6 +133,9 @@
     </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -408,10 +417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -454,6 +463,17 @@
         <v>5</v>
       </c>
     </row>
+    <row r="4" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="4">
+        <v>44232</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>